<commit_message>
Added clarifying questions to prompt in Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt_Chart.xlsx
+++ b/Gantt_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parke\Data_Science_Class\final-project-spencer_parker_chris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7113B188-CDE9-437C-B6E4-8DB2E9823B8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9562EF57-E01E-4F67-B7ED-8DB5DDDA9949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08D10644-7DC5-43F1-B54C-B6E5B1A722C3}"/>
   </bookViews>
@@ -82,13 +82,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -117,10 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -136,6 +143,102 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89547726-4951-4E14-AB90-E64E7896E750}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="323850" y="2571749"/>
+          <a:ext cx="5130800" cy="1628776"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>How does different food, group feeding, and location affect how often the sharks take food, target, drop food, or fast? Is there a pattern we can see on the individual or group level? Is there an optimal mix of food that gives us the best response? Are there any correlations between food types and location with light training, water temperature, or time of year? Focus on optimal mix of food that is the best for feeding</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> (focus on different ratios and their outcomes) What can we do to get our sharks to feed the best? Focus on the effects of food additives (Does the presence of vitamins or garlic change feeding habits?) </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -435,15 +538,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE291F45-733C-4102-ABBA-4A60E2EA047C}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="11" max="11" width="8.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -465,58 +571,60 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G8" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>